<commit_message>
make prepare figure function
</commit_message>
<xml_diff>
--- a/example_files/custom-scenario-table-template-complex-with-inputs-in-orange-and-defaults-in-gray.xlsx
+++ b/example_files/custom-scenario-table-template-complex-with-inputs-in-orange-and-defaults-in-gray.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/projects/PyLoopKit/example_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FEDA09E-06FB-3946-BA0C-D64D02549C6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB7F3CF-032B-654E-BCDC-32392CAA88C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="27240" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1060,10 +1060,10 @@
   <dimension ref="A1:EI46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1751,13 +1751,13 @@
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1844,7 +1844,7 @@
       <c r="E34" s="5">
         <v>43692.533449074072</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update order of rows in template
</commit_message>
<xml_diff>
--- a/example_files/custom-scenario-table-template-complex-with-inputs-in-orange-and-defaults-in-gray.xlsx
+++ b/example_files/custom-scenario-table-template-complex-with-inputs-in-orange-and-defaults-in-gray.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/projects/PyLoopKit/example_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB7F3CF-032B-654E-BCDC-32392CAA88C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9183004-9AFF-3743-A966-3C7B28B3F082}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="27240" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1060,10 +1060,10 @@
   <dimension ref="A1:EI46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1493,39 +1493,39 @@
     </row>
     <row r="2" spans="1:139">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:139">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:139">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>60</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:139">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:139">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>30</v>
@@ -1533,55 +1533,55 @@
     </row>
     <row r="7" spans="1:139">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4">
-        <v>15</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:139">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:139">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4">
-        <v>0.05</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:139">
       <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:139">
       <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="4">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:139">
       <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:139">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
         <v>10</v>
@@ -1589,18 +1589,18 @@
     </row>
     <row r="14" spans="1:139">
       <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:139">
       <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="4" t="b">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B15" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:139">
@@ -1611,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1619,344 +1619,344 @@
         <v>43692.512615740743</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="5">
+        <v>43692.512615740743</v>
+      </c>
+      <c r="E18" s="5">
+        <v>43692.533449074072</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C19" s="3">
         <v>0</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D19" s="3">
         <v>0.22916666666666666</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E19" s="3">
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C20" s="2">
         <v>330</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="2">
         <v>420</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E20" s="2">
         <v>650</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C21" s="2">
         <v>0.65</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D21" s="2">
         <v>0.9</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E21" s="2">
         <v>0.7</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="5">
-        <v>43692.5075</v>
-      </c>
-      <c r="D22" s="5">
-        <v>43692.507708333331</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="2">
+        <v>29</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="2">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2">
         <v>10</v>
       </c>
-      <c r="D23" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="2">
-        <v>120</v>
-      </c>
-      <c r="D24" s="2">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="E24" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>32</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
       </c>
       <c r="D26" s="3">
-        <v>0.47916666666666669</v>
+        <v>0.4375</v>
       </c>
       <c r="E26" s="3">
-        <v>0.70833333333333337</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="2">
-        <v>15</v>
-      </c>
-      <c r="D27" s="2">
-        <v>10</v>
-      </c>
-      <c r="E27" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>43</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>44</v>
+      </c>
+      <c r="C28" s="2">
+        <v>50</v>
+      </c>
+      <c r="D28" s="2">
+        <v>40</v>
+      </c>
+      <c r="E28" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>45</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="5">
-        <v>43692.507638888892</v>
-      </c>
-      <c r="D30" s="5">
-        <v>43692.507789351854</v>
-      </c>
-      <c r="E30" s="5">
-        <v>43692.509143518517</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>47</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="5">
-        <v>43692.508055555554</v>
-      </c>
-      <c r="D31" s="5">
-        <v>43692.50917824074</v>
-      </c>
-      <c r="E31" s="5">
-        <v>43692.512615740743</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>48</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C32" s="2">
-        <v>0.9</v>
+        <v>85</v>
       </c>
       <c r="D32" s="2">
-        <v>3</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:139">
       <c r="A33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>40</v>
+        <v>50</v>
+      </c>
+      <c r="C33" s="2">
+        <v>85</v>
+      </c>
+      <c r="D33" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:139">
       <c r="A34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="5">
-        <v>43692.512615740743</v>
-      </c>
-      <c r="E34" s="5">
-        <v>43692.533449074072</v>
-      </c>
-      <c r="F34" s="2">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:139">
       <c r="A35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0.4375</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0.75</v>
+        <v>24</v>
+      </c>
+      <c r="C35" s="5">
+        <v>43692.5075</v>
+      </c>
+      <c r="D35" s="5">
+        <v>43692.507708333331</v>
       </c>
     </row>
     <row r="36" spans="1:139">
       <c r="A36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="3">
-        <v>0.4375</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="E36" s="3">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="C36" s="2">
+        <v>10</v>
+      </c>
+      <c r="D36" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:139">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C37" s="2">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="D37" s="2">
-        <v>40</v>
-      </c>
-      <c r="E37" s="2">
-        <v>45</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:139">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:139">
       <c r="A39" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="3">
-        <v>0</v>
-      </c>
-      <c r="D39" s="3">
-        <v>0.5625</v>
+        <v>33</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:139">
       <c r="A40" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="3">
-        <v>0.5625</v>
-      </c>
-      <c r="D40" s="3">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="C40" s="5">
+        <v>43692.507638888892</v>
+      </c>
+      <c r="D40" s="5">
+        <v>43692.507789351854</v>
+      </c>
+      <c r="E40" s="5">
+        <v>43692.509143518517</v>
       </c>
     </row>
     <row r="41" spans="1:139">
       <c r="A41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="2">
-        <v>85</v>
-      </c>
-      <c r="D41" s="2">
-        <v>100</v>
+        <v>37</v>
+      </c>
+      <c r="C41" s="5">
+        <v>43692.508055555554</v>
+      </c>
+      <c r="D41" s="5">
+        <v>43692.50917824074</v>
+      </c>
+      <c r="E41" s="5">
+        <v>43692.512615740743</v>
       </c>
     </row>
     <row r="42" spans="1:139">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C42" s="2">
-        <v>85</v>
+        <v>0.9</v>
       </c>
       <c r="D42" s="2">
-        <v>100</v>
+        <v>3</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:139">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:139">

</xml_diff>